<commit_message>
Changed the Excel file and generated new schema
Changed the way dependencies are represented in Excel file and regenerated the schema to meet the new representation
</commit_message>
<xml_diff>
--- a/Json Schema/OSW_Tags.xlsx
+++ b/Json Schema/OSW_Tags.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MAGDEBURG\SURESH\oswvalidators\Json Schema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AEAE524-F78A-46DA-9B46-744F68BB9438}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B462CA95-2C79-4378-85E2-9EB593525AC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parents" sheetId="4" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="118">
   <si>
     <t>Tag</t>
   </si>
@@ -416,13 +416,64 @@
     </r>
   </si>
   <si>
-    <t>ChildTag</t>
-  </si>
-  <si>
     <t>DEPENDENCIES:</t>
   </si>
   <si>
     <t>Define each dependency on a new line for now</t>
+  </si>
+  <si>
+    <t>highway=footway</t>
+  </si>
+  <si>
+    <t>footway=crossing</t>
+  </si>
+  <si>
+    <t>footway=kerb_raised</t>
+  </si>
+  <si>
+    <t>footway=sidewalk</t>
+  </si>
+  <si>
+    <t>crossing=marked</t>
+  </si>
+  <si>
+    <t>crossing=unmarked</t>
+  </si>
+  <si>
+    <t>crossing=island</t>
+  </si>
+  <si>
+    <t>barrier=kerb</t>
+  </si>
+  <si>
+    <t>barrier=tactile_paving</t>
+  </si>
+  <si>
+    <t>barrier=amenity</t>
+  </si>
+  <si>
+    <t>barrier=power</t>
+  </si>
+  <si>
+    <t>traffic_signals=foot</t>
+  </si>
+  <si>
+    <t>traffic_signals=timing</t>
+  </si>
+  <si>
+    <t>traffic_signals=sound</t>
+  </si>
+  <si>
+    <t>traffic_signals=vibration</t>
+  </si>
+  <si>
+    <t>traffic_signals=button_operated</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>Prereqs</t>
   </si>
 </sst>
 </file>
@@ -739,18 +790,18 @@
   </sheetPr>
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -766,55 +817,55 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>4</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>7</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>16</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>16</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>16</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -822,102 +873,78 @@
         <v>32</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>4</v>
+        <v>103</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>17</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>4</v>
+        <v>103</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>17</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>4</v>
+        <v>103</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>17</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>4</v>
+        <v>103</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>17</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
         <v>93</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>4</v>
+        <v>103</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>17</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>4</v>
+        <v>103</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>17</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
@@ -964,7 +991,7 @@
         <v>24</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>63</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -972,7 +999,7 @@
         <v>67</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>63</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -980,7 +1007,7 @@
         <v>68</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>63</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -988,7 +1015,7 @@
         <v>72</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1052,7 +1079,7 @@
         <v>93</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>22</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
@@ -1060,7 +1087,7 @@
         <v>92</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>22</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
@@ -1068,7 +1095,7 @@
         <v>89</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>22</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
@@ -1076,7 +1103,7 @@
         <v>90</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>22</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
@@ -1084,7 +1111,7 @@
         <v>91</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>22</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1094,13 +1121,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:L1003"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1123,7 +1150,7 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1161,7 +1188,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1181,7 +1208,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
@@ -1204,7 +1231,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -1222,7 +1249,7 @@
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:12" ht="12.6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" ht="12.6" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
@@ -1245,7 +1272,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
@@ -1262,7 +1289,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
@@ -1279,7 +1306,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
@@ -1296,7 +1323,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
         <v>22</v>
       </c>
@@ -1313,7 +1340,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
         <v>32</v>
       </c>
@@ -1345,7 +1372,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
         <v>40</v>
       </c>
@@ -1359,7 +1386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="3" t="s">
         <v>42</v>
       </c>
@@ -1376,7 +1403,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
         <v>43</v>
       </c>
@@ -1390,7 +1417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="7" t="s">
         <v>44</v>
       </c>
@@ -1411,7 +1438,7 @@
       </c>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="7" t="s">
         <v>46</v>
       </c>
@@ -1432,7 +1459,7 @@
       </c>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -1455,7 +1482,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
         <v>51</v>
       </c>
@@ -1469,7 +1496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="3" t="s">
         <v>53</v>
       </c>
@@ -1492,7 +1519,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="3" t="s">
         <v>58</v>
       </c>
@@ -1512,7 +1539,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3" t="s">
         <v>62</v>
       </c>
@@ -1551,8 +1578,11 @@
       <c r="G22" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="H22" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
         <v>24</v>
       </c>
@@ -1575,7 +1605,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="3" t="s">
         <v>67</v>
       </c>
@@ -1592,7 +1622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="3" t="s">
         <v>68</v>
       </c>
@@ -1612,7 +1642,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="3" t="s">
         <v>72</v>
       </c>
@@ -1626,7 +1656,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="3" t="s">
         <v>74</v>
       </c>
@@ -1640,7 +1670,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="12.3" hidden="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A28" s="3" t="s">
         <v>76</v>
       </c>
@@ -1654,7 +1684,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="12.3" hidden="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A29" s="3" t="s">
         <v>78</v>
       </c>
@@ -1674,7 +1704,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="12.3" hidden="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A30" s="3" t="s">
         <v>79</v>
       </c>
@@ -1691,7 +1721,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="12.3" hidden="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A31" s="3" t="s">
         <v>80</v>
       </c>
@@ -1717,7 +1747,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="12.3" hidden="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A32" s="3" t="s">
         <v>87</v>
       </c>
@@ -1777,7 +1807,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="12.3" hidden="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A35" s="7" t="s">
         <v>92</v>
       </c>
@@ -1791,7 +1821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="12.3" hidden="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A36" s="3" t="s">
         <v>89</v>
       </c>
@@ -1811,7 +1841,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="12.3" hidden="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A37" s="3" t="s">
         <v>90</v>
       </c>
@@ -1831,7 +1861,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="12.3" hidden="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A38" s="3" t="s">
         <v>91</v>
       </c>
@@ -4747,20 +4777,6 @@
       <c r="C1003" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L38" xr:uid="{210F1B32-8683-4F65-85C3-79AF47DE39F5}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="barrier"/>
-        <filter val="foot"/>
-        <filter val="traffic_signals"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Point"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <dataValidations count="2">
     <dataValidation type="custom" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="C1" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>NOT(ISERROR(SEARCH(("type"),(C1))))</formula1>
@@ -4781,7 +4797,7 @@
   </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -4807,12 +4823,12 @@
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Schema generation and errors fixed
</commit_message>
<xml_diff>
--- a/Json Schema/OSW_Tags.xlsx
+++ b/Json Schema/OSW_Tags.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MAGDEBURG\SURESH\oswvalidators\Json Schema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B462CA95-2C79-4378-85E2-9EB593525AC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BCB75E8-3DCC-4D3D-85FB-4C87BC3CEA25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,8 @@
     <sheet name="Legend" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tags!$A$1:$L$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Parents!$A$1:$C$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tags!$A$1:$L$32</definedName>
   </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
@@ -30,7 +31,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -45,7 +46,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A35" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="A29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -66,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="97">
   <si>
     <t>Tag</t>
   </si>
@@ -131,9 +132,6 @@
     <t>unmarked</t>
   </si>
   <si>
-    <t>island</t>
-  </si>
-  <si>
     <t>traffic_signals</t>
   </si>
   <si>
@@ -212,9 +210,6 @@
     <t>alley</t>
   </si>
   <si>
-    <t>crossover</t>
-  </si>
-  <si>
     <t>driveway</t>
   </si>
   <si>
@@ -224,24 +219,6 @@
     <t>level</t>
   </si>
   <si>
-    <t>LineString, Point</t>
-  </si>
-  <si>
-    <t>smoothness</t>
-  </si>
-  <si>
-    <t>excellent</t>
-  </si>
-  <si>
-    <t>good</t>
-  </si>
-  <si>
-    <t>intermediate</t>
-  </si>
-  <si>
-    <t>bad</t>
-  </si>
-  <si>
     <t>brunnel</t>
   </si>
   <si>
@@ -260,15 +237,6 @@
     <t>barrier</t>
   </si>
   <si>
-    <t>hedge</t>
-  </si>
-  <si>
-    <t>wall</t>
-  </si>
-  <si>
-    <t>fence</t>
-  </si>
-  <si>
     <t>tactile_paving</t>
   </si>
   <si>
@@ -296,21 +264,9 @@
     <t>fire_hydrant</t>
   </si>
   <si>
-    <t>junction</t>
-  </si>
-  <si>
-    <t>roundabout</t>
-  </si>
-  <si>
     <t>manhole</t>
   </si>
   <si>
-    <t>shape</t>
-  </si>
-  <si>
-    <t>material</t>
-  </si>
-  <si>
     <t>rectangular</t>
   </si>
   <si>
@@ -330,24 +286,6 @@
   </si>
   <si>
     <t>public_transportation</t>
-  </si>
-  <si>
-    <t>stop_position</t>
-  </si>
-  <si>
-    <t>sound</t>
-  </si>
-  <si>
-    <t>vibration</t>
-  </si>
-  <si>
-    <t>button_operated</t>
-  </si>
-  <si>
-    <t>timing</t>
-  </si>
-  <si>
-    <t>foot</t>
   </si>
   <si>
     <t>None</t>
@@ -428,52 +366,52 @@
     <t>footway=crossing</t>
   </si>
   <si>
-    <t>footway=kerb_raised</t>
-  </si>
-  <si>
     <t>footway=sidewalk</t>
   </si>
   <si>
-    <t>crossing=marked</t>
-  </si>
-  <si>
-    <t>crossing=unmarked</t>
-  </si>
-  <si>
-    <t>crossing=island</t>
-  </si>
-  <si>
     <t>barrier=kerb</t>
   </si>
   <si>
-    <t>barrier=tactile_paving</t>
-  </si>
-  <si>
-    <t>barrier=amenity</t>
-  </si>
-  <si>
-    <t>barrier=power</t>
-  </si>
-  <si>
-    <t>traffic_signals=foot</t>
-  </si>
-  <si>
-    <t>traffic_signals=timing</t>
-  </si>
-  <si>
-    <t>traffic_signals=sound</t>
-  </si>
-  <si>
-    <t>traffic_signals=vibration</t>
-  </si>
-  <si>
-    <t>traffic_signals=button_operated</t>
-  </si>
-  <si>
     <t>Tags</t>
   </si>
   <si>
     <t>Prereqs</t>
+  </si>
+  <si>
+    <t>traffic_signals:foot=yes</t>
+  </si>
+  <si>
+    <t>traffic_signals:timing</t>
+  </si>
+  <si>
+    <t>traffic_signals:sound</t>
+  </si>
+  <si>
+    <t>traffic_signals:vibration</t>
+  </si>
+  <si>
+    <t>traffic_signals:button_operated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">crossing:island </t>
+  </si>
+  <si>
+    <t>highway=service</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>crossing:island</t>
+  </si>
+  <si>
+    <t>manhole:shape</t>
+  </si>
+  <si>
+    <t>manhole:material</t>
+  </si>
+  <si>
+    <t>traffic_signals:foot</t>
   </si>
 </sst>
 </file>
@@ -785,23 +723,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0E96FBC-F060-424C-8A71-1DB253C988CD}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="18.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>116</v>
+        <v>83</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -809,7 +750,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -817,7 +758,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -825,7 +766,7 @@
         <v>17</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -833,288 +774,212 @@
         <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
-        <v>18</v>
+        <v>90</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>104</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>105</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>106</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>101</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+        <v>73</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="3" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+        <v>73</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
-        <v>93</v>
+        <v>55</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+        <v>73</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+        <v>82</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>94</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A19" s="3" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A20" s="3" t="s">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A21" s="3" t="s">
-        <v>24</v>
+        <v>86</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A24" s="3" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="A28" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="A29" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="A30" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="A31" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="A32" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="A33" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="A34" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="A35" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="A36" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C24" xr:uid="{668CFC27-8C72-4858-804F-B63637471B96}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="barrier=amenity"/>
+        <filter val="barrier=kerb"/>
+        <filter val="barrier=power"/>
+        <filter val="barrier=tactile_paving"/>
+        <filter val="crossing=island"/>
+        <filter val="crossing=marked"/>
+        <filter val="crossing=unmarked"/>
+        <filter val="footway=crossing"/>
+        <filter val="footway=kerb_raised"/>
+        <filter val="footway=sidewalk"/>
+        <filter val="highway=footway"/>
+        <filter val="traffic_signals=button_operated"/>
+        <filter val="traffic_signals=foot"/>
+        <filter val="traffic_signals=sound"/>
+        <filter val="traffic_signals=timing"/>
+        <filter val="traffic_signals=vibration"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1124,15 +989,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L1003"/>
+  <dimension ref="A1:L997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="19.109375" customWidth="1"/>
+    <col min="1" max="1" width="18.71875" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1205,7 +1072,7 @@
         <v>17</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>18</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1224,12 +1091,8 @@
       <c r="E4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
@@ -1239,7 +1102,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="4">
         <v>0</v>
@@ -1251,30 +1114,30 @@
     </row>
     <row r="6" spans="1:12" ht="12.6" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
-        <v>19</v>
+        <v>93</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>5</v>
@@ -1283,15 +1146,18 @@
         <v>6</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>31</v>
+      <c r="F7" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>5</v>
@@ -1300,15 +1166,15 @@
         <v>6</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>5</v>
@@ -1317,109 +1183,117 @@
         <v>6</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="D11" s="7">
+        <v>-90</v>
+      </c>
+      <c r="E11" s="3">
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="3" t="s">
-        <v>42</v>
+      <c r="A13" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="7">
-        <v>-90</v>
-      </c>
-      <c r="E13" s="3">
-        <v>90</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="3" t="s">
-        <v>43</v>
+      <c r="A14" s="7" t="s">
+        <v>45</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="7">
-        <v>0</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="7" t="s">
-        <v>44</v>
+      <c r="A15" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>5</v>
@@ -1428,487 +1302,376 @@
         <v>6</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="7" t="s">
-        <v>46</v>
+      <c r="A16" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>45</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>50</v>
+        <v>22</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="3">
-        <v>0</v>
+      <c r="F18" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>57</v>
+        <v>22</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="3">
-        <v>0</v>
-      </c>
-      <c r="E21" s="3">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E22" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="3">
-        <v>0</v>
-      </c>
-      <c r="E24" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+        <v>6</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A25" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A26" s="3" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+        <v>66</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A27" s="3" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>75</v>
+        <v>68</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A28" s="3" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>77</v>
+        <v>29</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="A29" s="3" t="s">
-        <v>78</v>
+      <c r="A29" s="7" t="s">
+        <v>86</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>67</v>
+        <v>22</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A30" s="3" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>81</v>
+        <v>29</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>82</v>
+        <v>30</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A31" s="3" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>83</v>
+        <v>29</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>84</v>
+        <v>30</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>86</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A32" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="A33" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="A34" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E34" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="A35" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D35" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="A36" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="A37" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="A38" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="F32" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="C33" s="8"/>
+    </row>
+    <row r="34" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="C34" s="8"/>
+    </row>
+    <row r="35" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="C35" s="8"/>
+    </row>
+    <row r="36" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="C36" s="8"/>
+    </row>
+    <row r="37" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="C37" s="8"/>
+    </row>
+    <row r="38" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="C38" s="8"/>
+    </row>
+    <row r="39" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C39" s="8"/>
     </row>
-    <row r="40" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="40" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C40" s="8"/>
     </row>
-    <row r="41" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="41" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C41" s="8"/>
     </row>
-    <row r="42" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="42" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C42" s="8"/>
     </row>
-    <row r="43" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="43" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C43" s="8"/>
     </row>
-    <row r="44" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="44" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C44" s="8"/>
     </row>
-    <row r="45" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="45" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C45" s="8"/>
     </row>
-    <row r="46" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="46" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C46" s="8"/>
     </row>
-    <row r="47" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="47" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C47" s="8"/>
     </row>
-    <row r="48" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="48" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C48" s="8"/>
     </row>
     <row r="49" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
@@ -4757,31 +4520,13 @@
     </row>
     <row r="997" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C997" s="8"/>
-    </row>
-    <row r="998" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="C998" s="8"/>
-    </row>
-    <row r="999" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="C999" s="8"/>
-    </row>
-    <row r="1000" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="C1000" s="8"/>
-    </row>
-    <row r="1001" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="C1001" s="8"/>
-    </row>
-    <row r="1002" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="C1002" s="8"/>
-    </row>
-    <row r="1003" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="C1003" s="8"/>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="custom" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="C1" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>NOT(ISERROR(SEARCH(("type"),(C1))))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2:C1003" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2:C997" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"string,integer,number,boolean"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4808,27 +4553,27 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B1" s="3" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="3" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="3" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="9" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="10" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Generated correct nodes schema
Generated Correct nodes schema.
Added additional error message for "anyOf"
</commit_message>
<xml_diff>
--- a/Json Schema/OSW_Tags.xlsx
+++ b/Json Schema/OSW_Tags.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MAGDEBURG\SURESH\oswvalidators\Json Schema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BCB75E8-3DCC-4D3D-85FB-4C87BC3CEA25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D53C1D-C260-4817-8226-719CC930C9CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parents" sheetId="4" r:id="rId1"/>
@@ -728,8 +728,8 @@
   </sheetPr>
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:C16"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -991,8 +991,8 @@
   </sheetPr>
   <dimension ref="A1:L997"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Modified Tags information and test cases
After the call with Suresh, made the error information more user friendly
</commit_message>
<xml_diff>
--- a/Json Schema/OSW_Tags.xlsx
+++ b/Json Schema/OSW_Tags.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MAGDEBURG\SURESH\oswvalidators\Json Schema\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rakesh\Downloads\for_raki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D53C1D-C260-4817-8226-719CC930C9CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A8CFA6-DF92-4779-A566-05D2671D5CFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parents" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Parents!$A$1:$C$24</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tags!$A$1:$L$32</definedName>
   </definedNames>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -38,6 +38,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Couldn't find this tag in OSM.
 	-Rakesh kumar
@@ -53,6 +54,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>What is this used for?
 Is it any positive decimal or positive number? like natural number?
@@ -67,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="106">
   <si>
     <t>Tag</t>
   </si>
@@ -299,6 +301,7 @@
         <b/>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>string</t>
     </r>
@@ -307,6 +310,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>", then, the "values" are entries in the enum list for the string type. Only those values are allowed</t>
     </r>
@@ -320,6 +324,7 @@
         <b/>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>integer</t>
     </r>
@@ -328,6 +333,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>", the first value column is the minimum value allowed for the integer, the second value column if present, is the maximum value allowed</t>
     </r>
@@ -341,6 +347,7 @@
         <b/>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>number</t>
     </r>
@@ -349,6 +356,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>"</t>
     </r>
@@ -408,10 +416,37 @@
     <t>manhole:shape</t>
   </si>
   <si>
-    <t>manhole:material</t>
-  </si>
-  <si>
     <t>traffic_signals:foot</t>
+  </si>
+  <si>
+    <t>drain</t>
+  </si>
+  <si>
+    <t>sewer</t>
+  </si>
+  <si>
+    <t>telecom</t>
+  </si>
+  <si>
+    <t>public_transport</t>
+  </si>
+  <si>
+    <t>amenity=manhole</t>
+  </si>
+  <si>
+    <t>platform=yes</t>
+  </si>
+  <si>
+    <t>highway=path</t>
+  </si>
+  <si>
+    <t>highway=pedestrian</t>
+  </si>
+  <si>
+    <t>material</t>
+  </si>
+  <si>
+    <t>highway=traffic_signals</t>
   </si>
 </sst>
 </file>
@@ -429,16 +464,19 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -449,6 +487,7 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -723,21 +762,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0E96FBC-F060-424C-8A71-1DB253C988CD}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="18.5546875" customWidth="1"/>
+    <col min="2" max="2" width="20.71875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>83</v>
       </c>
@@ -745,7 +785,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -753,7 +793,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -761,7 +801,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
@@ -769,7 +809,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
@@ -777,7 +817,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
         <v>90</v>
       </c>
@@ -785,7 +825,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
         <v>31</v>
       </c>
@@ -798,7 +838,7 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
         <v>39</v>
       </c>
@@ -811,7 +851,7 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
         <v>41</v>
       </c>
@@ -821,10 +861,14 @@
       <c r="C9" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D9" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
         <v>42</v>
       </c>
@@ -837,7 +881,7 @@
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
@@ -848,7 +892,7 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
         <v>49</v>
       </c>
@@ -856,7 +900,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="3" t="s">
         <v>50</v>
       </c>
@@ -864,7 +908,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
         <v>55</v>
       </c>
@@ -872,7 +916,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
         <v>23</v>
       </c>
@@ -880,7 +924,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
         <v>56</v>
       </c>
@@ -890,10 +934,17 @@
       <c r="C16" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D16" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
         <v>57</v>
       </c>
@@ -901,7 +952,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
         <v>61</v>
       </c>
@@ -909,7 +960,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A19" s="3" t="s">
         <v>72</v>
       </c>
@@ -917,15 +968,15 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:3" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A20" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A21" s="3" t="s">
         <v>86</v>
       </c>
@@ -933,7 +984,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:3" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
         <v>87</v>
       </c>
@@ -941,7 +992,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:3" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
         <v>88</v>
       </c>
@@ -949,7 +1000,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A24" s="3" t="s">
         <v>89</v>
       </c>
@@ -957,29 +1008,17 @@
         <v>85</v>
       </c>
     </row>
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" s="3"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C24" xr:uid="{668CFC27-8C72-4858-804F-B63637471B96}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="barrier=amenity"/>
-        <filter val="barrier=kerb"/>
-        <filter val="barrier=power"/>
-        <filter val="barrier=tactile_paving"/>
-        <filter val="crossing=island"/>
-        <filter val="crossing=marked"/>
-        <filter val="crossing=unmarked"/>
-        <filter val="footway=crossing"/>
-        <filter val="footway=kerb_raised"/>
-        <filter val="footway=sidewalk"/>
-        <filter val="highway=footway"/>
-        <filter val="traffic_signals=button_operated"/>
-        <filter val="traffic_signals=foot"/>
-        <filter val="traffic_signals=sound"/>
-        <filter val="traffic_signals=timing"/>
-        <filter val="traffic_signals=vibration"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:C24" xr:uid="{668CFC27-8C72-4858-804F-B63637471B96}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -991,8 +1030,8 @@
   </sheetPr>
   <dimension ref="A1:L997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1329,7 +1368,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
         <v>49</v>
       </c>
@@ -1343,7 +1382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
         <v>50</v>
       </c>
@@ -1363,7 +1402,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="3" t="s">
         <v>54</v>
       </c>
@@ -1380,7 +1419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="3" t="s">
         <v>55</v>
       </c>
@@ -1398,7 +1437,7 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3" t="s">
         <v>56</v>
       </c>
@@ -1406,19 +1445,17 @@
         <v>5</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+        <v>22</v>
+      </c>
+      <c r="D21" s="3">
+        <v>1</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
         <v>57</v>
       </c>
@@ -1441,7 +1478,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
         <v>61</v>
       </c>
@@ -1455,7 +1492,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="3" t="s">
         <v>63</v>
       </c>
@@ -1469,7 +1506,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:9" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A25" s="3" t="s">
         <v>65</v>
       </c>
@@ -1483,13 +1520,22 @@
         <v>29</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
+        <v>61</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A26" s="3" t="s">
         <v>94</v>
       </c>
@@ -1506,9 +1552,9 @@
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:9" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A27" s="3" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>24</v>
@@ -1532,9 +1578,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:9" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A28" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>24</v>
@@ -1552,7 +1598,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:9" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A29" s="7" t="s">
         <v>86</v>
       </c>
@@ -1566,7 +1612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:9" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A30" s="3" t="s">
         <v>87</v>
       </c>
@@ -1586,7 +1632,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:9" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A31" s="3" t="s">
         <v>88</v>
       </c>
@@ -1606,7 +1652,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:9" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A32" s="3" t="s">
         <v>89</v>
       </c>
@@ -1626,52 +1672,63 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="C33" s="8"/>
-    </row>
-    <row r="34" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:4" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A33" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C34" s="8"/>
     </row>
-    <row r="35" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:4" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C35" s="8"/>
     </row>
-    <row r="36" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:4" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C36" s="8"/>
     </row>
-    <row r="37" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:4" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C37" s="8"/>
     </row>
-    <row r="38" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:4" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C38" s="8"/>
     </row>
-    <row r="39" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:4" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C39" s="8"/>
     </row>
-    <row r="40" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:4" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C40" s="8"/>
     </row>
-    <row r="41" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:4" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C41" s="8"/>
     </row>
-    <row r="42" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:4" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C42" s="8"/>
     </row>
-    <row r="43" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:4" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C43" s="8"/>
     </row>
-    <row r="44" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:4" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C44" s="8"/>
     </row>
-    <row r="45" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:4" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C45" s="8"/>
     </row>
-    <row r="46" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:4" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C46" s="8"/>
     </row>
-    <row r="47" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:4" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C47" s="8"/>
     </row>
-    <row r="48" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:4" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C48" s="8"/>
     </row>
     <row r="49" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">

</xml_diff>